<commit_message>
begin travel recommender script
</commit_message>
<xml_diff>
--- a/Travel_Destinations.xlsx
+++ b/Travel_Destinations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\swe_dev\personal_projects\travel_recommendation_engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94ABE62E-7107-42E9-9345-60C289582B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85526CD2-63F4-4866-8C9C-0826295C9D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{421A95C2-6272-4696-AA38-ACAEF6D352DA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
   <si>
     <t>India</t>
   </si>
@@ -744,9 +744,6 @@
   </si>
   <si>
     <t>Côte d’Ivoire</t>
-  </si>
-  <si>
-    <t>Vatican City</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F0DC90-7EB3-41D8-8F16-743D55E68686}">
-  <dimension ref="A1:A237"/>
+  <dimension ref="A1:A236"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
       <selection activeCell="A237" sqref="A237"/>
@@ -2295,11 +2292,6 @@
         <v>232</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A237" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>